<commit_message>
Se agregan los primeros resultados del Test snowflake to python
</commit_message>
<xml_diff>
--- a/Test_Tablas_conciliacion_PBI.xlsx
+++ b/Test_Tablas_conciliacion_PBI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\git_project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CE4408-6524-445E-961E-9DA0DDD3F9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3EE93F-382B-47B2-8839-3E9CEA46566B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="403" xr2:uid="{4225C3A4-0CEB-4E5F-A412-E7E42CF40BC7}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="En revision" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Directorio!$A$1:$K$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Directorio!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>País</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>CO_KUSHKI_TEST</t>
+  </si>
+  <si>
+    <t>archivo_resultado_excel</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -225,6 +228,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -540,27 +544,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33530C62-835C-476F-95DF-E49FEB8931C0}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="77.7109375" customWidth="1"/>
-    <col min="11" max="11" width="52.7109375" customWidth="1"/>
+    <col min="10" max="10" width="75.5703125" customWidth="1"/>
+    <col min="11" max="11" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -594,8 +603,11 @@
       <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,44 +636,49 @@
         <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;H2&amp;".csv"</f>
         <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/CO_KUSHKI_TEST.csv</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="str">
+        <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;H2&amp;".xlsx"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/CO_KUSHKI_TEST.xlsx</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E5" s="5"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="7:9" x14ac:dyDescent="0.25">
@@ -852,7 +869,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K55" xr:uid="{33530C62-835C-476F-95DF-E49FEB8931C0}"/>
+  <autoFilter ref="A1:L1" xr:uid="{33530C62-835C-476F-95DF-E49FEB8931C0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Se incluyen las carpetas y los cambios de la tablas_conciliacion
</commit_message>
<xml_diff>
--- a/Test_Tablas_conciliacion_PBI.xlsx
+++ b/Test_Tablas_conciliacion_PBI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\git_project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3EE93F-382B-47B2-8839-3E9CEA46566B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C712D4F0-2659-4FF0-914C-059E8732ED98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="403" xr2:uid="{4225C3A4-0CEB-4E5F-A412-E7E42CF40BC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="403" xr2:uid="{4225C3A4-0CEB-4E5F-A412-E7E42CF40BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Directorio" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>País</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>archivo_resultado_excel</t>
+  </si>
+  <si>
+    <t>CO_WOMPI_CONC_MAN_VEN</t>
+  </si>
+  <si>
+    <t>CO_WOMPI_CONC_SIM_VEN</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
 </sst>
 </file>
@@ -547,10 +559,10 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +581,7 @@
     <col min="12" max="12" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -615,13 +627,13 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H2" t="str">
         <f>E2</f>
@@ -633,19 +645,79 @@
         <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_KUSHKI_TEST.sql</v>
       </c>
       <c r="K2" t="str">
-        <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;H2&amp;".csv"</f>
-        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/CO_KUSHKI_TEST.csv</v>
+        <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;C2&amp;"/"&amp;H2&amp;".csv"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_KUSHKI_TEST.csv</v>
       </c>
       <c r="L2" t="str">
-        <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;H2&amp;".xlsx"</f>
-        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/CO_KUSHKI_TEST.xlsx</v>
+        <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;C2&amp;"/"&amp;H2&amp;".xlsx"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_KUSHKI_TEST.xlsx</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
       <c r="I3" s="4"/>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J4" si="0">"C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/"&amp;B3&amp;"/"&amp;E3&amp;".sql"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_WOMPI_CONC_MAN_VEN.sql</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K4" si="1">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B3&amp;"/"&amp;C3&amp;"/"&amp;H3&amp;".csv"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_WOMPI_CONC_MAN_VEN.csv</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L4" si="2">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B3&amp;"/"&amp;C3&amp;"/"&amp;H3&amp;".xlsx"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_WOMPI_CONC_MAN_VEN.xlsx</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
       <c r="I4" s="4"/>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_WOMPI_CONC_SIM_VEN.sql</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/SIM/CO_WOMPI_CONC_SIM_VEN.csv</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/SIM/CO_WOMPI_CONC_SIM_VEN.xlsx</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E5" s="5"/>
@@ -835,11 +907,11 @@
         <v>21</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" ref="J54:J55" si="0">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;E54&amp;".sql"</f>
+        <f t="shared" ref="J54:J55" si="3">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;E54&amp;".sql"</f>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/PE/PE_RAPPICARD_CONC_VEN.sql</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" ref="K54:K55" si="1">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;H54&amp;".xlsx"</f>
+        <f t="shared" ref="K54:K55" si="4">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;H54&amp;".xlsx"</f>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/PE/PE_VISANET.xlsx</v>
       </c>
     </row>
@@ -860,11 +932,11 @@
         <v>26</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/MX/MX_RAPPICARD_CONC_VEN.sql</v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/MX/MX_RAPPICARD.xlsx</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se incluyen querys parametricos de Colombia
</commit_message>
<xml_diff>
--- a/Test_Tablas_conciliacion_PBI.xlsx
+++ b/Test_Tablas_conciliacion_PBI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\git_project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C712D4F0-2659-4FF0-914C-059E8732ED98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9359996-A943-47FA-A692-F18EB9F6D7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="403" xr2:uid="{4225C3A4-0CEB-4E5F-A412-E7E42CF40BC7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
   <si>
     <t>País</t>
   </si>
@@ -140,6 +140,42 @@
   </si>
   <si>
     <t>SIM</t>
+  </si>
+  <si>
+    <t>BR_ADYEN_CONC_MAN_VEN_REF</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>BR_ADYEN</t>
+  </si>
+  <si>
+    <t>CO_WOMPI_CONC_SIM_VEN_REF</t>
+  </si>
+  <si>
+    <t>CO_WOMPI</t>
+  </si>
+  <si>
+    <t>CO_BANCOLOMBIA_CONC_MAN_REF</t>
+  </si>
+  <si>
+    <t>CO_BANCOLOMBIA</t>
+  </si>
+  <si>
+    <t>CO_RAPPICARD_CONC_MAN_VEN</t>
+  </si>
+  <si>
+    <t>CO_RAPPICARD</t>
+  </si>
+  <si>
+    <t>CO_RAPPICARD_CONC_MAN_REF</t>
+  </si>
+  <si>
+    <t>CO_RAPPICARD_CONC_MAN_REF_INV</t>
+  </si>
+  <si>
+    <t>CO_RAPPICARD_CONC_MAN_VEN_INV</t>
   </si>
 </sst>
 </file>
@@ -228,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +277,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -559,10 +597,10 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2:L4"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,8 +614,8 @@
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="75.5703125" customWidth="1"/>
-    <col min="11" max="11" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="97" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="98.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -645,8 +683,8 @@
         <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_KUSHKI_TEST.sql</v>
       </c>
       <c r="K2" t="str">
-        <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;C2&amp;"/"&amp;H2&amp;".csv"</f>
-        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_KUSHKI_TEST.csv</v>
+        <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;C2&amp;"/"&amp;H2</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_KUSHKI_TEST</v>
       </c>
       <c r="L2" t="str">
         <f>"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B2&amp;"/"&amp;C2&amp;"/"&amp;H2&amp;".xlsx"</f>
@@ -667,22 +705,22 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J4" si="0">"C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/"&amp;B3&amp;"/"&amp;E3&amp;".sql"</f>
+        <f t="shared" ref="J3:J9" si="0">"C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/"&amp;B3&amp;"/"&amp;E3&amp;".sql"</f>
         <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_WOMPI_CONC_MAN_VEN.sql</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K4" si="1">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B3&amp;"/"&amp;C3&amp;"/"&amp;H3&amp;".csv"</f>
-        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_WOMPI_CONC_MAN_VEN.csv</v>
+        <f t="shared" ref="K3:K5" si="1">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B3&amp;"/"&amp;C3&amp;"/"&amp;H3</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_WOMPI_CONC_MAN_VEN</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L4" si="2">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B3&amp;"/"&amp;C3&amp;"/"&amp;H3&amp;".xlsx"</f>
+        <f t="shared" ref="L3:L5" si="2">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B3&amp;"/"&amp;C3&amp;"/"&amp;H3&amp;".xlsx"</f>
         <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_WOMPI_CONC_MAN_VEN.xlsx</v>
       </c>
     </row>
@@ -700,7 +738,7 @@
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -712,7 +750,7 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/SIM/CO_WOMPI_CONC_SIM_VEN.csv</v>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/SIM/CO_WOMPI_CONC_SIM_VEN</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="2"/>
@@ -720,23 +758,236 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="5"/>
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="I5" s="4"/>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/BR/BR_ADYEN_CONC_MAN_VEN_REF.sql</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/BR/MAN/BR_ADYEN</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/BR/MAN/BR_ADYEN.xlsx</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="4"/>
+      <c r="H6" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="I6" s="4"/>
+      <c r="J6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_WOMPI_CONC_SIM_VEN_REF.sql</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" ref="K6:K9" si="3">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B6&amp;"/"&amp;C6&amp;"/"&amp;H6</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/SIM/CO_WOMPI</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" ref="L6:L11" si="4">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B6&amp;"/"&amp;C6&amp;"/"&amp;H6&amp;".xlsx"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/SIM/CO_WOMPI.xlsx</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="4"/>
+      <c r="H7" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="I7" s="4"/>
+      <c r="J7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_BANCOLOMBIA_CONC_MAN_REF.sql</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_BANCOLOMBIA</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="4"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_BANCOLOMBIA.xlsx</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_RAPPICARD_CONC_MAN_VEN.sql</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="4"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD.xlsx</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_RAPPICARD_CONC_MAN_REF.sql</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="3"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="4"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD.xlsx</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="G10" s="4"/>
+      <c r="H10" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="I10" s="4"/>
+      <c r="J10" s="7" t="str">
+        <f t="shared" ref="J10:J11" si="5">"C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/"&amp;B10&amp;"/"&amp;E10&amp;".sql"</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_RAPPICARD_CONC_MAN_VEN_INV.sql</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" ref="K10:K11" si="6">"C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/"&amp;B10&amp;"/"&amp;C10&amp;"/"&amp;H10</f>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="4"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD.xlsx</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="I11" s="4"/>
+      <c r="J11" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/QUERY_SQL/CO/CO_RAPPICARD_CONC_MAN_REF_INV.sql</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="6"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="4"/>
+        <v>C:/Users/Usuario/Desktop/git_project_1/Fuente_Power_BI/CO/MAN/CO_RAPPICARD.xlsx</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="4"/>
@@ -907,11 +1158,11 @@
         <v>21</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" ref="J54:J55" si="3">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;E54&amp;".sql"</f>
+        <f t="shared" ref="J54:J55" si="7">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;E54&amp;".sql"</f>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/PE/PE_RAPPICARD_CONC_VEN.sql</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" ref="K54:K55" si="4">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;H54&amp;".xlsx"</f>
+        <f t="shared" ref="K54:K55" si="8">"G:/Mi unidad/Query_SQL/Autom_cierre/"&amp;B54&amp;"/"&amp;H54&amp;".xlsx"</f>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/PE/PE_VISANET.xlsx</v>
       </c>
     </row>
@@ -932,11 +1183,11 @@
         <v>26</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/MX/MX_RAPPICARD_CONC_VEN.sql</v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>G:/Mi unidad/Query_SQL/Autom_cierre/MX/MX_RAPPICARD.xlsx</v>
       </c>
     </row>

</xml_diff>